<commit_message>
changed 6, 9, ab=nd 10
</commit_message>
<xml_diff>
--- a/dbms/Problems 1.xlsx
+++ b/dbms/Problems 1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="205">
   <si>
     <t>}</t>
   </si>
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t>SEASON, HOTEL</t>
-  </si>
-  <si>
-    <t>Получится пустое множество</t>
   </si>
   <si>
     <t>A6</t>
@@ -1407,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N166" sqref="N166"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2598,14 +2595,18 @@
       <c r="D108" s="19"/>
     </row>
     <row r="109" spans="1:11">
-      <c r="B109" s="19" t="s">
-        <v>200</v>
+      <c r="B109" s="21">
+        <v>3</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="19"/>
     </row>
     <row r="110" spans="1:11">
-      <c r="B110"/>
+      <c r="B110" s="21">
+        <v>17</v>
+      </c>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
     </row>
     <row r="111" spans="1:11">
       <c r="A111">
@@ -2928,7 +2929,7 @@
         <v>37</v>
       </c>
       <c r="N158" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P158" s="38"/>
       <c r="Q158" s="43"/>
@@ -2960,7 +2961,7 @@
         <v>40</v>
       </c>
       <c r="N159" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P159" s="38"/>
       <c r="Q159" s="43"/>
@@ -2995,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="P160" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q160" s="32"/>
       <c r="R160" s="32"/>
@@ -3029,7 +3030,7 @@
         <v>1</v>
       </c>
       <c r="P161" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q161" s="32"/>
       <c r="R161" s="32"/>
@@ -3063,7 +3064,7 @@
         <v>2</v>
       </c>
       <c r="P162" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q162" s="32"/>
       <c r="R162" s="32"/>

</xml_diff>